<commit_message>
Revised L21 and comments on math_self_efficacy data
</commit_message>
<xml_diff>
--- a/data/math_self_efficacy.xlsx
+++ b/data/math_self_efficacy.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\craigaj\Downloads\Temp data folder\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\craigaj\Documents\GitHub\M221R\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29855ADE-363A-4E84-9C90-796168FD9E8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0CDC922-79FD-44FD-90C3-CB95BF45593F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-8205" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,35 +33,17 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="34">
   <si>
     <t>F</t>
   </si>
   <si>
-    <t>Shane Goodwin and other researchers studied factors that affect a student's confidence</t>
-  </si>
-  <si>
-    <t>on a multiple-choice Mathematics exam. A group of n = 139 students in an Intermediate</t>
-  </si>
-  <si>
     <t>Algebra course at BYU-Idaho participated in the study.</t>
   </si>
   <si>
     <t/>
   </si>
   <si>
-    <t>The exam consisted of 30 multiple-choice problems worth a total of 100 points.</t>
-  </si>
-  <si>
-    <t>The students' scores out of 100 points are given in the variable "Scores."</t>
-  </si>
-  <si>
-    <t>For each test question, the students evaluated their confidence in their response</t>
-  </si>
-  <si>
-    <t>on a scale of 1 to 6.</t>
-  </si>
-  <si>
     <t>Confidence Rating Scale:</t>
   </si>
   <si>
@@ -120,6 +102,39 @@
   </si>
   <si>
     <t>comments</t>
+  </si>
+  <si>
+    <t>on a multiple-choice Mathematics exam.</t>
+  </si>
+  <si>
+    <t>A group of n = 139 students in an Intermediate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The exam consisted of 30 multiple-choice </t>
+  </si>
+  <si>
+    <t>problems worth a total of 100 points.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The students' scores out of 100 points </t>
+  </si>
+  <si>
+    <t>are given in the variable "Scores."</t>
+  </si>
+  <si>
+    <t>factors that affect a student's confidence</t>
+  </si>
+  <si>
+    <t>Shane Goodwin and other researchers studied</t>
+  </si>
+  <si>
+    <t xml:space="preserve">For each test question, the students </t>
+  </si>
+  <si>
+    <t xml:space="preserve">evaluated their confidence in their </t>
+  </si>
+  <si>
+    <t>response on a scale of 1 to 6.</t>
   </si>
 </sst>
 </file>
@@ -498,7 +513,7 @@
   <dimension ref="A1:D140"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="D16" sqref="D16:D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -508,16 +523,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="B1" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="C1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="D1" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
@@ -531,7 +546,7 @@
         <v>4.34</v>
       </c>
       <c r="D2" t="s">
-        <v>1</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
@@ -545,7 +560,7 @@
         <v>4.7300000000000004</v>
       </c>
       <c r="D3" t="s">
-        <v>2</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
@@ -559,7 +574,7 @@
         <v>5.28</v>
       </c>
       <c r="D4" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
@@ -573,7 +588,7 @@
         <v>2.83</v>
       </c>
       <c r="D5" t="s">
-        <v>4</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
@@ -587,7 +602,7 @@
         <v>5.4</v>
       </c>
       <c r="D6" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
@@ -601,7 +616,7 @@
         <v>4.03</v>
       </c>
       <c r="D7" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
@@ -615,7 +630,7 @@
         <v>4.9000000000000004</v>
       </c>
       <c r="D8" t="s">
-        <v>4</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
@@ -629,7 +644,7 @@
         <v>5.93</v>
       </c>
       <c r="D9" t="s">
-        <v>7</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
@@ -643,7 +658,7 @@
         <v>3.89</v>
       </c>
       <c r="D10" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
@@ -657,7 +672,7 @@
         <v>2.48</v>
       </c>
       <c r="D11" t="s">
-        <v>4</v>
+        <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
@@ -671,7 +686,7 @@
         <v>3.53</v>
       </c>
       <c r="D12" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
@@ -685,7 +700,7 @@
         <v>5.27</v>
       </c>
       <c r="D13" t="s">
-        <v>10</v>
+        <v>31</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
@@ -699,7 +714,7 @@
         <v>2.37</v>
       </c>
       <c r="D14" t="s">
-        <v>11</v>
+        <v>32</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.35">
@@ -713,7 +728,7 @@
         <v>4.3099999999999996</v>
       </c>
       <c r="D15" t="s">
-        <v>12</v>
+        <v>33</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.35">
@@ -726,9 +741,6 @@
       <c r="C16">
         <v>5.33</v>
       </c>
-      <c r="D16" t="s">
-        <v>13</v>
-      </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
@@ -741,7 +753,7 @@
         <v>4.13</v>
       </c>
       <c r="D17" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.35">
@@ -755,7 +767,7 @@
         <v>5.7</v>
       </c>
       <c r="D18" t="s">
-        <v>15</v>
+        <v>4</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.35">
@@ -769,7 +781,7 @@
         <v>5.17</v>
       </c>
       <c r="D19" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.35">
@@ -783,7 +795,7 @@
         <v>4.33</v>
       </c>
       <c r="D20" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.35">
@@ -797,7 +809,7 @@
         <v>5.33</v>
       </c>
       <c r="D21" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.35">
@@ -811,7 +823,7 @@
         <v>3.83</v>
       </c>
       <c r="D22" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.35">
@@ -825,7 +837,7 @@
         <v>4.93</v>
       </c>
       <c r="D23" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.35">
@@ -839,7 +851,7 @@
         <v>4.57</v>
       </c>
       <c r="D24" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.35">
@@ -853,7 +865,7 @@
         <v>4.07</v>
       </c>
       <c r="D25" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.35">
@@ -867,7 +879,7 @@
         <v>3.37</v>
       </c>
       <c r="D26" t="s">
-        <v>21</v>
+        <v>2</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.35">
@@ -881,7 +893,7 @@
         <v>4.4000000000000004</v>
       </c>
       <c r="D27" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.35">
@@ -895,7 +907,7 @@
         <v>2</v>
       </c>
       <c r="D28" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.35">
@@ -909,7 +921,7 @@
         <v>3.57</v>
       </c>
       <c r="D29" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.35">
@@ -923,7 +935,7 @@
         <v>4.5999999999999996</v>
       </c>
       <c r="D30" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.35">
@@ -937,7 +949,7 @@
         <v>3.4</v>
       </c>
       <c r="D31" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.35">
@@ -951,7 +963,7 @@
         <v>3.72</v>
       </c>
       <c r="D32" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.35">
@@ -965,7 +977,7 @@
         <v>4.1399999999999997</v>
       </c>
       <c r="D33" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.35">
@@ -979,7 +991,7 @@
         <v>4.17</v>
       </c>
       <c r="D34" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.35">
@@ -993,7 +1005,7 @@
         <v>4.3</v>
       </c>
       <c r="D35" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.35">
@@ -1007,7 +1019,7 @@
         <v>2.35</v>
       </c>
       <c r="D36" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.35">
@@ -1021,7 +1033,7 @@
         <v>4.63</v>
       </c>
       <c r="D37" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.35">
@@ -1035,7 +1047,7 @@
         <v>3.9</v>
       </c>
       <c r="D38" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.35">
@@ -1049,7 +1061,7 @@
         <v>3.73</v>
       </c>
       <c r="D39" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.35">
@@ -1063,7 +1075,7 @@
         <v>4.43</v>
       </c>
       <c r="D40" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.35">
@@ -1077,7 +1089,7 @@
         <v>5.53</v>
       </c>
       <c r="D41" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.35">
@@ -1091,7 +1103,7 @@
         <v>5.43</v>
       </c>
       <c r="D42" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.35">
@@ -1105,7 +1117,7 @@
         <v>4.37</v>
       </c>
       <c r="D43" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.35">
@@ -1119,7 +1131,7 @@
         <v>3.8</v>
       </c>
       <c r="D44" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.35">
@@ -1133,7 +1145,7 @@
         <v>4.7300000000000004</v>
       </c>
       <c r="D45" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.35">
@@ -1147,7 +1159,7 @@
         <v>4.6900000000000004</v>
       </c>
       <c r="D46" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.35">
@@ -1161,7 +1173,7 @@
         <v>4.13</v>
       </c>
       <c r="D47" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.35">
@@ -1175,7 +1187,7 @@
         <v>5.3</v>
       </c>
       <c r="D48" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.35">
@@ -1189,7 +1201,7 @@
         <v>5.03</v>
       </c>
       <c r="D49" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.35">
@@ -1203,7 +1215,7 @@
         <v>3.79</v>
       </c>
       <c r="D50" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.35">
@@ -1217,7 +1229,7 @@
         <v>4.47</v>
       </c>
       <c r="D51" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.35">
@@ -1231,7 +1243,7 @@
         <v>4.47</v>
       </c>
       <c r="D52" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.35">
@@ -1245,7 +1257,7 @@
         <v>2.77</v>
       </c>
       <c r="D53" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.35">
@@ -1259,7 +1271,7 @@
         <v>4.2</v>
       </c>
       <c r="D54" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.35">
@@ -1273,7 +1285,7 @@
         <v>5.33</v>
       </c>
       <c r="D55" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.35">
@@ -1287,7 +1299,7 @@
         <v>3.83</v>
       </c>
       <c r="D56" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.35">
@@ -1301,7 +1313,7 @@
         <v>5.5</v>
       </c>
       <c r="D57" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.35">
@@ -1315,7 +1327,7 @@
         <v>4.67</v>
       </c>
       <c r="D58" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.35">
@@ -1329,7 +1341,7 @@
         <v>5.13</v>
       </c>
       <c r="D59" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.35">
@@ -1343,7 +1355,7 @@
         <v>4.5</v>
       </c>
       <c r="D60" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.35">
@@ -1357,7 +1369,7 @@
         <v>5.5</v>
       </c>
       <c r="D61" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.35">
@@ -1371,7 +1383,7 @@
         <v>3.21</v>
       </c>
       <c r="D62" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.35">
@@ -1385,7 +1397,7 @@
         <v>5.5</v>
       </c>
       <c r="D63" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.35">
@@ -1399,7 +1411,7 @@
         <v>4.37</v>
       </c>
       <c r="D64" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.35">
@@ -1413,12 +1425,12 @@
         <v>4.1100000000000003</v>
       </c>
       <c r="D65" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B66">
         <v>53.3</v>
@@ -1427,12 +1439,12 @@
         <v>4.17</v>
       </c>
       <c r="D66" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B67">
         <v>70</v>
@@ -1441,12 +1453,12 @@
         <v>4.12</v>
       </c>
       <c r="D67" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B68">
         <v>90</v>
@@ -1455,12 +1467,12 @@
         <v>4.7</v>
       </c>
       <c r="D68" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B69">
         <v>93.3</v>
@@ -1469,12 +1481,12 @@
         <v>5</v>
       </c>
       <c r="D69" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B70">
         <v>83.3</v>
@@ -1483,12 +1495,12 @@
         <v>5.41</v>
       </c>
       <c r="D70" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B71">
         <v>63.3</v>
@@ -1497,12 +1509,12 @@
         <v>3.03</v>
       </c>
       <c r="D71" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B72">
         <v>50</v>
@@ -1511,12 +1523,12 @@
         <v>3.47</v>
       </c>
       <c r="D72" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B73">
         <v>60</v>
@@ -1525,12 +1537,12 @@
         <v>1.57</v>
       </c>
       <c r="D73" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B74">
         <v>73.3</v>
@@ -1539,12 +1551,12 @@
         <v>3.2</v>
       </c>
       <c r="D74" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B75">
         <v>36.700000000000003</v>
@@ -1553,12 +1565,12 @@
         <v>3</v>
       </c>
       <c r="D75" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B76">
         <v>93.3</v>
@@ -1567,12 +1579,12 @@
         <v>5.67</v>
       </c>
       <c r="D76" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B77">
         <v>83.3</v>
@@ -1581,12 +1593,12 @@
         <v>4.43</v>
       </c>
       <c r="D77" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B78">
         <v>73.3</v>
@@ -1595,12 +1607,12 @@
         <v>5.0999999999999996</v>
       </c>
       <c r="D78" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B79">
         <v>56.7</v>
@@ -1609,12 +1621,12 @@
         <v>3.28</v>
       </c>
       <c r="D79" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B80">
         <v>96.7</v>
@@ -1623,12 +1635,12 @@
         <v>6</v>
       </c>
       <c r="D80" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B81">
         <v>70</v>
@@ -1637,12 +1649,12 @@
         <v>5.4</v>
       </c>
       <c r="D81" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B82">
         <v>66.7</v>
@@ -1651,12 +1663,12 @@
         <v>3.9</v>
       </c>
       <c r="D82" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B83">
         <v>66.7</v>
@@ -1665,12 +1677,12 @@
         <v>3.67</v>
       </c>
       <c r="D83" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B84">
         <v>83.3</v>
@@ -1679,12 +1691,12 @@
         <v>4.33</v>
       </c>
       <c r="D84" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B85">
         <v>93.3</v>
@@ -1693,12 +1705,12 @@
         <v>5.87</v>
       </c>
       <c r="D85" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B86">
         <v>90</v>
@@ -1707,12 +1719,12 @@
         <v>5.31</v>
       </c>
       <c r="D86" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B87">
         <v>93.3</v>
@@ -1721,12 +1733,12 @@
         <v>4.5999999999999996</v>
       </c>
       <c r="D87" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B88">
         <v>83.3</v>
@@ -1735,12 +1747,12 @@
         <v>5.97</v>
       </c>
       <c r="D88" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B89">
         <v>83.3</v>
@@ -1749,12 +1761,12 @@
         <v>4.2699999999999996</v>
       </c>
       <c r="D89" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B90">
         <v>43.3</v>
@@ -1763,12 +1775,12 @@
         <v>4.5599999999999996</v>
       </c>
       <c r="D90" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B91">
         <v>63.3</v>
@@ -1777,12 +1789,12 @@
         <v>4.2300000000000004</v>
       </c>
       <c r="D91" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B92">
         <v>93.3</v>
@@ -1791,12 +1803,12 @@
         <v>4.9000000000000004</v>
       </c>
       <c r="D92" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B93">
         <v>66.7</v>
@@ -1805,12 +1817,12 @@
         <v>4.83</v>
       </c>
       <c r="D93" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B94">
         <v>56.7</v>
@@ -1819,12 +1831,12 @@
         <v>2.52</v>
       </c>
       <c r="D94" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B95">
         <v>56.7</v>
@@ -1833,12 +1845,12 @@
         <v>4.59</v>
       </c>
       <c r="D95" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B96">
         <v>73.3</v>
@@ -1847,12 +1859,12 @@
         <v>3.12</v>
       </c>
       <c r="D96" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B97">
         <v>93.3</v>
@@ -1861,12 +1873,12 @@
         <v>5.77</v>
       </c>
       <c r="D97" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B98">
         <v>66.7</v>
@@ -1875,12 +1887,12 @@
         <v>4.43</v>
       </c>
       <c r="D98" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B99">
         <v>100</v>
@@ -1889,12 +1901,12 @@
         <v>5.2</v>
       </c>
       <c r="D99" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B100">
         <v>86.7</v>
@@ -1903,12 +1915,12 @@
         <v>5.6</v>
       </c>
       <c r="D100" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B101">
         <v>43.3</v>
@@ -1917,12 +1929,12 @@
         <v>2.37</v>
       </c>
       <c r="D101" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B102">
         <v>73.3</v>
@@ -1931,12 +1943,12 @@
         <v>4.8</v>
       </c>
       <c r="D102" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B103">
         <v>63.3</v>
@@ -1945,12 +1957,12 @@
         <v>4.62</v>
       </c>
       <c r="D103" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B104">
         <v>40</v>
@@ -1959,12 +1971,12 @@
         <v>3.53</v>
       </c>
       <c r="D104" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B105">
         <v>43.3</v>
@@ -1973,12 +1985,12 @@
         <v>2.61</v>
       </c>
       <c r="D105" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B106">
         <v>73.3</v>
@@ -1987,12 +1999,12 @@
         <v>3.45</v>
       </c>
       <c r="D106" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B107">
         <v>90</v>
@@ -2001,12 +2013,12 @@
         <v>4.5999999999999996</v>
       </c>
       <c r="D107" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B108">
         <v>93.3</v>
@@ -2015,12 +2027,12 @@
         <v>6</v>
       </c>
       <c r="D108" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B109">
         <v>76.7</v>
@@ -2029,12 +2041,12 @@
         <v>4.93</v>
       </c>
       <c r="D109" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B110">
         <v>86.7</v>
@@ -2043,12 +2055,12 @@
         <v>5.17</v>
       </c>
       <c r="D110" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B111">
         <v>80</v>
@@ -2057,12 +2069,12 @@
         <v>4.33</v>
       </c>
       <c r="D111" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B112">
         <v>76.7</v>
@@ -2071,12 +2083,12 @@
         <v>5.37</v>
       </c>
       <c r="D112" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B113">
         <v>53.3</v>
@@ -2085,12 +2097,12 @@
         <v>3.62</v>
       </c>
       <c r="D113" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B114">
         <v>93.3</v>
@@ -2099,12 +2111,12 @@
         <v>4.5</v>
       </c>
       <c r="D114" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B115">
         <v>76.7</v>
@@ -2113,12 +2125,12 @@
         <v>4.3099999999999996</v>
       </c>
       <c r="D115" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B116">
         <v>90</v>
@@ -2127,12 +2139,12 @@
         <v>5.33</v>
       </c>
       <c r="D116" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B117">
         <v>83.3</v>
@@ -2141,12 +2153,12 @@
         <v>4.7</v>
       </c>
       <c r="D117" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B118">
         <v>76.7</v>
@@ -2155,12 +2167,12 @@
         <v>3.3</v>
       </c>
       <c r="D118" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B119">
         <v>93.3</v>
@@ -2169,12 +2181,12 @@
         <v>5.73</v>
       </c>
       <c r="D119" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B120">
         <v>93.3</v>
@@ -2183,12 +2195,12 @@
         <v>4.93</v>
       </c>
       <c r="D120" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B121">
         <v>80</v>
@@ -2197,12 +2209,12 @@
         <v>3.83</v>
       </c>
       <c r="D121" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B122">
         <v>80</v>
@@ -2211,12 +2223,12 @@
         <v>5.13</v>
       </c>
       <c r="D122" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B123">
         <v>86.7</v>
@@ -2225,12 +2237,12 @@
         <v>5.67</v>
       </c>
       <c r="D123" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B124">
         <v>70</v>
@@ -2239,12 +2251,12 @@
         <v>4.87</v>
       </c>
       <c r="D124" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B125">
         <v>76.7</v>
@@ -2253,12 +2265,12 @@
         <v>4.1500000000000004</v>
       </c>
       <c r="D125" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B126">
         <v>73.3</v>
@@ -2267,12 +2279,12 @@
         <v>4.37</v>
       </c>
       <c r="D126" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B127">
         <v>56.7</v>
@@ -2281,12 +2293,12 @@
         <v>3.36</v>
       </c>
       <c r="D127" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B128">
         <v>90</v>
@@ -2295,12 +2307,12 @@
         <v>5.17</v>
       </c>
       <c r="D128" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B129">
         <v>76.7</v>
@@ -2309,12 +2321,12 @@
         <v>4.37</v>
       </c>
       <c r="D129" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A130" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B130">
         <v>90</v>
@@ -2323,12 +2335,12 @@
         <v>5.2</v>
       </c>
       <c r="D130" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A131" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B131">
         <v>53.3</v>
@@ -2337,12 +2349,12 @@
         <v>3.4</v>
       </c>
       <c r="D131" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A132" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B132">
         <v>36.700000000000003</v>
@@ -2351,12 +2363,12 @@
         <v>3.34</v>
       </c>
       <c r="D132" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A133" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B133">
         <v>83.3</v>
@@ -2365,12 +2377,12 @@
         <v>4.04</v>
       </c>
       <c r="D133" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A134" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B134">
         <v>73.3</v>
@@ -2379,12 +2391,12 @@
         <v>4.2699999999999996</v>
       </c>
       <c r="D134" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A135" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B135">
         <v>86.7</v>
@@ -2393,12 +2405,12 @@
         <v>5.43</v>
       </c>
       <c r="D135" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A136" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B136">
         <v>86.7</v>
@@ -2406,13 +2418,10 @@
       <c r="C136">
         <v>5.83</v>
       </c>
-      <c r="D136" t="s">
-        <v>4</v>
-      </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A137" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B137">
         <v>90</v>
@@ -2420,13 +2429,10 @@
       <c r="C137">
         <v>5.77</v>
       </c>
-      <c r="D137" t="s">
-        <v>4</v>
-      </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A138" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B138">
         <v>96.7</v>
@@ -2434,13 +2440,10 @@
       <c r="C138">
         <v>5.8</v>
       </c>
-      <c r="D138" t="s">
-        <v>4</v>
-      </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A139" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B139">
         <v>76.7</v>
@@ -2448,22 +2451,16 @@
       <c r="C139">
         <v>4.5999999999999996</v>
       </c>
-      <c r="D139" t="s">
-        <v>4</v>
-      </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B140">
         <v>70</v>
       </c>
       <c r="C140">
         <v>3.77</v>
-      </c>
-      <c r="D140" t="s">
-        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>